<commit_message>
A bunch of bug fixes in invoice submissions
</commit_message>
<xml_diff>
--- a/invoices.xlsx
+++ b/invoices.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming Projects\ASN_Sub_Automator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A4F58BA-A5F8-42C8-B039-CEAD08BCC72D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC600362-19BC-4650-B971-AF4C3C54A9E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="15800" xr2:uid="{453091CF-8C07-4572-BCA9-6CBB294DFA3A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>PO</t>
   </si>
@@ -50,39 +50,160 @@
     <t>Total</t>
   </si>
   <si>
-    <t>42XTOQKA</t>
-  </si>
-  <si>
-    <t>7EW99H1D</t>
-  </si>
-  <si>
-    <t>737IK4IE</t>
-  </si>
-  <si>
-    <t>7FO8Z58J</t>
-  </si>
-  <si>
-    <t>2WIDAODD</t>
-  </si>
-  <si>
-    <t>2R4IXG3K</t>
-  </si>
-  <si>
-    <t>17G8QD8Q</t>
-  </si>
-  <si>
-    <t>1ABWW2SN</t>
-  </si>
-  <si>
-    <t>2YD4VS8S</t>
+    <t>8S2FCAAU</t>
+  </si>
+  <si>
+    <t>3736LUUY</t>
+  </si>
+  <si>
+    <t>198OVCFA</t>
+  </si>
+  <si>
+    <t>7Y9861LW</t>
+  </si>
+  <si>
+    <t>75FT9HIJ</t>
+  </si>
+  <si>
+    <t>29PM6XLH</t>
+  </si>
+  <si>
+    <t>3VQLPUWR</t>
+  </si>
+  <si>
+    <t>7RXPML9K</t>
+  </si>
+  <si>
+    <t>1GBY5ZEF</t>
+  </si>
+  <si>
+    <t>7TSH8P4Z</t>
+  </si>
+  <si>
+    <t>3XRGHHQO</t>
+  </si>
+  <si>
+    <t>89P72C5T</t>
+  </si>
+  <si>
+    <t>1I3TEF4J</t>
+  </si>
+  <si>
+    <t>787RPCOY</t>
+  </si>
+  <si>
+    <t>8IDETXJJ</t>
+  </si>
+  <si>
+    <t>82IW3UAY</t>
+  </si>
+  <si>
+    <t>1S2328GX</t>
+  </si>
+  <si>
+    <t>49UNLEKB</t>
+  </si>
+  <si>
+    <t>4OQ97QZM</t>
+  </si>
+  <si>
+    <t>5ZQ2SSJU</t>
+  </si>
+  <si>
+    <t>3VAH57CZ</t>
+  </si>
+  <si>
+    <t>1LHKGUDK</t>
+  </si>
+  <si>
+    <t>1DKRY5YH</t>
+  </si>
+  <si>
+    <t>15WHWBBO</t>
+  </si>
+  <si>
+    <t>4L1PZJAI</t>
+  </si>
+  <si>
+    <t>7231GHCV</t>
+  </si>
+  <si>
+    <t>67RV4UPD</t>
+  </si>
+  <si>
+    <t>3LF1TUYL</t>
+  </si>
+  <si>
+    <t>5WXWXO4U</t>
+  </si>
+  <si>
+    <t>8Q6MQSHL</t>
+  </si>
+  <si>
+    <t>2OXTRO2E</t>
+  </si>
+  <si>
+    <t>4ZDL8JEV</t>
+  </si>
+  <si>
+    <t>66ZVE7IX</t>
+  </si>
+  <si>
+    <t>85GFKESW</t>
+  </si>
+  <si>
+    <t>8SMAX2KY</t>
+  </si>
+  <si>
+    <t>74D2E1UA</t>
+  </si>
+  <si>
+    <t>4B6DPF3F</t>
+  </si>
+  <si>
+    <t>7OJYK5ZJ</t>
+  </si>
+  <si>
+    <t>8QVK32VO</t>
+  </si>
+  <si>
+    <t>511VVBWT</t>
+  </si>
+  <si>
+    <t>8K5HN6HH</t>
+  </si>
+  <si>
+    <t>1TI65UPY</t>
+  </si>
+  <si>
+    <t>5ER5W17F</t>
+  </si>
+  <si>
+    <t>28L8SWJV</t>
+  </si>
+  <si>
+    <t>3PQ7BURG</t>
+  </si>
+  <si>
+    <t>56ACM54O</t>
+  </si>
+  <si>
+    <t>5IGO48WJ</t>
+  </si>
+  <si>
+    <t>1HEQ1G2O</t>
+  </si>
+  <si>
+    <t>4JW39TSA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="m/d/yyyy;@"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="m/d/yyyy;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -113,8 +234,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -450,10 +572,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57100417-66A6-4AEE-A68A-166723D26E93}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -461,7 +583,8 @@
     <col min="1" max="1" width="11.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.75" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -474,134 +597,694 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="B2" s="1">
-        <v>45725</v>
+        <v>45743</v>
       </c>
       <c r="C2">
-        <v>9907</v>
-      </c>
-      <c r="D2">
-        <v>56.16</v>
+        <v>9962</v>
+      </c>
+      <c r="D2" s="2">
+        <v>379.67</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="B3" s="1">
-        <v>45725</v>
+        <v>45743</v>
       </c>
       <c r="C3">
-        <v>9914</v>
-      </c>
-      <c r="D3">
-        <v>442.52</v>
+        <v>9963</v>
+      </c>
+      <c r="D3" s="2">
+        <v>80.849999999999994</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="B4" s="1">
-        <v>45725</v>
+        <v>45743</v>
       </c>
       <c r="C4">
-        <v>9926</v>
-      </c>
-      <c r="D4">
-        <v>322</v>
+        <v>9964</v>
+      </c>
+      <c r="D4" s="2">
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="B5" s="1">
-        <v>45725</v>
+        <v>45743</v>
       </c>
       <c r="C5">
-        <v>9927</v>
-      </c>
-      <c r="D5">
-        <v>108.68</v>
+        <v>9965</v>
+      </c>
+      <c r="D5" s="2">
+        <v>194</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="B6" s="1">
-        <v>45725</v>
+        <v>45743</v>
       </c>
       <c r="C6">
-        <v>9928</v>
-      </c>
-      <c r="D6">
-        <v>418.8</v>
+        <v>9966</v>
+      </c>
+      <c r="D6" s="2">
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="B7" s="1">
-        <v>45725</v>
+        <v>45743</v>
       </c>
       <c r="C7">
-        <v>9929</v>
-      </c>
-      <c r="D7">
-        <v>306.75</v>
+        <v>9967</v>
+      </c>
+      <c r="D7" s="2">
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="B8" s="1">
-        <v>45725</v>
+        <v>45743</v>
       </c>
       <c r="C8">
-        <v>9930</v>
-      </c>
-      <c r="D8">
-        <v>34.200000000000003</v>
+        <v>9968</v>
+      </c>
+      <c r="D8" s="2">
+        <v>712.86</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="B9" s="1">
-        <v>45725</v>
+        <v>45743</v>
       </c>
       <c r="C9">
-        <v>9931</v>
-      </c>
-      <c r="D9">
-        <v>247.5</v>
+        <v>9969</v>
+      </c>
+      <c r="D9" s="2">
+        <v>262.2</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="1">
+        <v>45743</v>
+      </c>
+      <c r="C10">
+        <v>9970</v>
+      </c>
+      <c r="D10" s="2">
+        <v>108.68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="1">
+        <v>45743</v>
+      </c>
+      <c r="C11">
+        <v>9971</v>
+      </c>
+      <c r="D11" s="2">
+        <v>108.68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="1">
+        <v>45743</v>
+      </c>
+      <c r="C12">
+        <v>9972</v>
+      </c>
+      <c r="D12" s="2">
+        <v>713.29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="1">
+        <v>45743</v>
+      </c>
+      <c r="C13">
+        <v>9973</v>
+      </c>
+      <c r="D13" s="2">
+        <v>108.68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="1">
+        <v>45743</v>
+      </c>
+      <c r="C14">
+        <v>9974</v>
+      </c>
+      <c r="D14" s="2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="1">
+        <v>45743</v>
+      </c>
+      <c r="C15">
+        <v>9975</v>
+      </c>
+      <c r="D15" s="2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="1">
+        <v>45743</v>
+      </c>
+      <c r="C16">
+        <v>9976</v>
+      </c>
+      <c r="D16" s="2">
+        <v>351.26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="1">
+        <v>45743</v>
+      </c>
+      <c r="C17">
+        <v>9977</v>
+      </c>
+      <c r="D17" s="2">
+        <v>261.41000000000003</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="1">
+        <v>45743</v>
+      </c>
+      <c r="C18">
+        <v>9978</v>
+      </c>
+      <c r="D18" s="2">
+        <v>108.68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="1">
+        <v>45743</v>
+      </c>
+      <c r="C19">
+        <v>9979</v>
+      </c>
+      <c r="D19" s="2">
+        <v>97.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" s="1">
+        <v>45743</v>
+      </c>
+      <c r="C20">
+        <v>9980</v>
+      </c>
+      <c r="D20" s="2">
+        <v>37.49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="1">
+        <v>45743</v>
+      </c>
+      <c r="C21">
+        <v>9981</v>
+      </c>
+      <c r="D21" s="2">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="1">
+        <v>45743</v>
+      </c>
+      <c r="C22">
+        <v>9982</v>
+      </c>
+      <c r="D22" s="2">
+        <v>336.88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="1">
+        <v>45743</v>
+      </c>
+      <c r="C23">
+        <v>9983</v>
+      </c>
+      <c r="D23" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="1">
+        <v>45743</v>
+      </c>
+      <c r="C24">
+        <v>9956</v>
+      </c>
+      <c r="D24" s="2">
+        <v>262.08</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="1">
+        <v>45743</v>
+      </c>
+      <c r="C25">
+        <v>9935</v>
+      </c>
+      <c r="D25" s="2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="1">
+        <v>45743</v>
+      </c>
+      <c r="C26">
+        <v>9936</v>
+      </c>
+      <c r="D26" s="2">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="1">
+        <v>45743</v>
+      </c>
+      <c r="C27">
+        <v>9937</v>
+      </c>
+      <c r="D27" s="2">
+        <v>610.14999999999986</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" s="1">
+        <v>45743</v>
+      </c>
+      <c r="C28">
+        <v>9938</v>
+      </c>
+      <c r="D28" s="2">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29" s="1">
+        <v>45743</v>
+      </c>
+      <c r="C29">
+        <v>9939</v>
+      </c>
+      <c r="D29" s="2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>9</v>
+      </c>
+      <c r="B30" s="1">
+        <v>45743</v>
+      </c>
+      <c r="C30">
+        <v>9940</v>
+      </c>
+      <c r="D30" s="2">
+        <v>111.6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>10</v>
+      </c>
+      <c r="B31" s="1">
+        <v>45743</v>
+      </c>
+      <c r="C31">
+        <v>9941</v>
+      </c>
+      <c r="D31" s="2">
+        <v>74.8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" s="1">
+        <v>45743</v>
+      </c>
+      <c r="C32">
+        <v>9942</v>
+      </c>
+      <c r="D32" s="2">
+        <v>209.9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="1">
-        <v>45725</v>
-      </c>
-      <c r="C10">
-        <v>9932</v>
-      </c>
-      <c r="D10">
-        <v>503.88</v>
+      <c r="B33" s="1">
+        <v>45743</v>
+      </c>
+      <c r="C33">
+        <v>9943</v>
+      </c>
+      <c r="D33" s="2">
+        <v>108.68</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" s="1">
+        <v>45743</v>
+      </c>
+      <c r="C34">
+        <v>9944</v>
+      </c>
+      <c r="D34" s="2">
+        <v>99.23</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35" s="1">
+        <v>45743</v>
+      </c>
+      <c r="C35">
+        <v>9945</v>
+      </c>
+      <c r="D35" s="2">
+        <v>97.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>15</v>
+      </c>
+      <c r="B36" s="1">
+        <v>45743</v>
+      </c>
+      <c r="C36">
+        <v>9946</v>
+      </c>
+      <c r="D36" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>16</v>
+      </c>
+      <c r="B37" s="1">
+        <v>45743</v>
+      </c>
+      <c r="C37">
+        <v>9947</v>
+      </c>
+      <c r="D37" s="2">
+        <v>1468</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>17</v>
+      </c>
+      <c r="B38" s="1">
+        <v>45743</v>
+      </c>
+      <c r="C38">
+        <v>9948</v>
+      </c>
+      <c r="D38" s="2">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>18</v>
+      </c>
+      <c r="B39" s="1">
+        <v>45743</v>
+      </c>
+      <c r="C39">
+        <v>9949</v>
+      </c>
+      <c r="D39" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>19</v>
+      </c>
+      <c r="B40" s="1">
+        <v>45743</v>
+      </c>
+      <c r="C40">
+        <v>9950</v>
+      </c>
+      <c r="D40" s="2">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>20</v>
+      </c>
+      <c r="B41" s="1">
+        <v>45743</v>
+      </c>
+      <c r="C41">
+        <v>9951</v>
+      </c>
+      <c r="D41" s="2">
+        <v>56.16</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>21</v>
+      </c>
+      <c r="B42" s="1">
+        <v>45743</v>
+      </c>
+      <c r="C42">
+        <v>9952</v>
+      </c>
+      <c r="D42" s="2">
+        <v>745.5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>22</v>
+      </c>
+      <c r="B43" s="1">
+        <v>45743</v>
+      </c>
+      <c r="C43">
+        <v>9953</v>
+      </c>
+      <c r="D43" s="2">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>23</v>
+      </c>
+      <c r="B44" s="1">
+        <v>45743</v>
+      </c>
+      <c r="C44">
+        <v>9954</v>
+      </c>
+      <c r="D44" s="2">
+        <v>379.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>24</v>
+      </c>
+      <c r="B45" s="1">
+        <v>45743</v>
+      </c>
+      <c r="C45">
+        <v>9955</v>
+      </c>
+      <c r="D45" s="2">
+        <v>97.5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>26</v>
+      </c>
+      <c r="B46" s="1">
+        <v>45743</v>
+      </c>
+      <c r="C46">
+        <v>9957</v>
+      </c>
+      <c r="D46" s="2">
+        <v>249.33</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>27</v>
+      </c>
+      <c r="B47" s="1">
+        <v>45743</v>
+      </c>
+      <c r="C47">
+        <v>9958</v>
+      </c>
+      <c r="D47" s="2">
+        <v>51.98</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>28</v>
+      </c>
+      <c r="B48" s="1">
+        <v>45743</v>
+      </c>
+      <c r="C48">
+        <v>9959</v>
+      </c>
+      <c r="D48" s="2">
+        <v>107.16</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>29</v>
+      </c>
+      <c r="B49" s="1">
+        <v>45743</v>
+      </c>
+      <c r="C49">
+        <v>9960</v>
+      </c>
+      <c r="D49" s="2">
+        <v>669.7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>30</v>
+      </c>
+      <c r="B50" s="1">
+        <v>45743</v>
+      </c>
+      <c r="C50">
+        <v>9961</v>
+      </c>
+      <c r="D50" s="2">
+        <v>108.68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>